<commit_message>
Added some dates and some time to the time sheet
</commit_message>
<xml_diff>
--- a/Time tracking sheet.xlsx
+++ b/Time tracking sheet.xlsx
@@ -8,24 +8,30 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\The project + with math\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D10D00C0-2458-4AAE-8890-EB382250578E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB9ADCE4-AFBF-4B55-9B9D-7D28C8724809}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Time keeping sheet for the group work</t>
   </si>
@@ -34,6 +40,18 @@
   </si>
   <si>
     <t>Jami</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>5-6 hours</t>
+  </si>
+  <si>
+    <t>project start some basic planning</t>
+  </si>
+  <si>
+    <t>bit of the 1,2 functions in javascript</t>
   </si>
 </sst>
 </file>
@@ -71,7 +89,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -352,10 +370,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -363,12 +381,15 @@
     <col min="1" max="20" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>3</v>
+      </c>
       <c r="B10" t="s">
         <v>1</v>
       </c>
@@ -376,8 +397,128 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>43801</v>
+      </c>
+      <c r="E11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>43802</v>
+      </c>
+      <c r="F12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>43803</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>43804</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>43805</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>43806</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>43807</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>43808</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>43809</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>43810</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>43811</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>43813</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>43814</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>43815</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>43816</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>43817</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>43818</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="1"/>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="1"/>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="1"/>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="1"/>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="1"/>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="1"/>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Made some changes to math and added Jalils combinations
</commit_message>
<xml_diff>
--- a/Time tracking sheet.xlsx
+++ b/Time tracking sheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\The project + with math\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB9ADCE4-AFBF-4B55-9B9D-7D28C8724809}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9BEEA7B-E241-4715-A13C-0DDEAEBD8E19}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Time keeping sheet for the group work</t>
   </si>
@@ -52,13 +52,28 @@
   </si>
   <si>
     <t>bit of the 1,2 functions in javascript</t>
+  </si>
+  <si>
+    <t>4 hours</t>
+  </si>
+  <si>
+    <t>2 hours</t>
+  </si>
+  <si>
+    <t>made the base for the banner</t>
+  </si>
+  <si>
+    <t>task 3basse work</t>
+  </si>
+  <si>
+    <t>end</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -66,13 +81,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -84,14 +111,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -370,10 +400,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -412,6 +442,9 @@
       <c r="A12" s="1">
         <v>43802</v>
       </c>
+      <c r="E12" t="s">
+        <v>7</v>
+      </c>
       <c r="F12" t="s">
         <v>6</v>
       </c>
@@ -420,92 +453,124 @@
       <c r="A13" s="1">
         <v>43803</v>
       </c>
+      <c r="E13" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>43804</v>
       </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>43805</v>
       </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>43806</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="E16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>43807</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="E17">
+        <v>2</v>
+      </c>
+      <c r="F17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>43808</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="E18">
+        <v>4</v>
+      </c>
+      <c r="F18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>43809</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>43810</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>43811</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>43812</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>43813</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>43814</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>43815</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>43816</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>43817</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
-        <v>43818</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>